<commit_message>
Bugfix Cell Style ExcelWriter
</commit_message>
<xml_diff>
--- a/ModernTest/ModernBaseLibrary/Data/ExcelWriter/DemoData/Demo_01.xlsx
+++ b/ModernTest/ModernBaseLibrary/Data/ExcelWriter/DemoData/Demo_01.xlsx
@@ -58,7 +58,7 @@
   <fills count="2">
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="00FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -105,7 +105,7 @@
         <v>123.789</v>
       </c>
       <c r="C2">
-        <v>45735.834641203706</v>
+        <v>45748.58043981482</v>
       </c>
       <c r="D2">
         <v>0.5350694444444445</v>

</xml_diff>